<commit_message>
Using pandas to load correction data.
</commit_message>
<xml_diff>
--- a/data/correction/template.xlsx
+++ b/data/correction/template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftDevelopment\Projects\IO Aero\io-avstats-db\data\correction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftDevelopment\Projects\IO-Aero\io-avstats\data\correction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D013BB-732F-4964-AC7C-9CBFF1F4701E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74A6F44-AE0B-4F53-8D00-C7063C378718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="0" windowWidth="25780" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -411,14 +411,14 @@
       <selection activeCell="H1" sqref="H1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="6"/>
+    <col min="5" max="7" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -450,7 +450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>